<commit_message>
Replaced Fig [1] & Modified AI Excel Sheet
</commit_message>
<xml_diff>
--- a/Documents/AI Excel sheet.xlsx
+++ b/Documents/AI Excel sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\Year 2 Term 2\AI Simulation Year 2\AI-Sim-Project\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Desktop\AI-Sim-Project\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9817A547-B7AA-477B-8170-E68C4124F1D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7647DF30-964C-40F1-B88C-102EE89B7253}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{4885B63F-A160-4F03-8E80-DC62420CED2B}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
   <si>
     <t>Date</t>
   </si>
@@ -170,9 +170,6 @@
     <t>Started generating pseudocode</t>
   </si>
   <si>
-    <t>Created FSM</t>
-  </si>
-  <si>
     <t>Started research on FSM</t>
   </si>
   <si>
@@ -204,6 +201,33 @@
   </si>
   <si>
     <t>Phil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retrospect = Did we do it </t>
+  </si>
+  <si>
+    <t>Sprint review = How well did we do it and what could be better</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>We successfully researched FSM using different sources and Looked at multiple strategies of implementation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We colour coded each week to correctly divide the different parts of the assignment plan, found no issues </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We created a lot of pseudocode for the FSM states, which we can now impliment into the project </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created rules for each of the states and the varying types of tanks </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We started the introduction with the explanation of the FSM with also the project management </t>
+  </si>
+  <si>
+    <t>Create OOP FSM</t>
   </si>
 </sst>
 </file>
@@ -1024,10 +1048,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB5E907D-8933-443F-B74A-7A0D16E3D46A}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,17 +1059,18 @@
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="97" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>32</v>
       </c>
@@ -1060,98 +1085,124 @@
       </c>
       <c r="E2" s="17"/>
       <c r="G2" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H2" s="17"/>
-    </row>
-    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="J2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>36</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
+        <v>47</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>61</v>
+      </c>
       <c r="G3" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="J3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="31"/>
       <c r="B4" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
+        <v>55</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>62</v>
+      </c>
       <c r="G4" s="17"/>
     </row>
-    <row r="5" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
+      <c r="C5" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>63</v>
+      </c>
       <c r="G5" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>38</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
+        <v>52</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>64</v>
+      </c>
       <c r="H6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
+        <v>51</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>65</v>
+      </c>
       <c r="H7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>39</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="20"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
+      <c r="B9" s="1"/>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
       <c r="B10" s="20"/>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>40</v>
       </c>
@@ -1159,7 +1210,7 @@
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>41</v>
       </c>
@@ -1167,7 +1218,7 @@
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>42</v>
       </c>
@@ -1175,7 +1226,7 @@
       <c r="C13" s="23"/>
       <c r="D13" s="23"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
         <v>43</v>
       </c>
@@ -1183,7 +1234,7 @@
       <c r="C14" s="24"/>
       <c r="D14" s="24"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>44</v>
       </c>
@@ -1191,7 +1242,7 @@
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
         <v>45</v>
       </c>
@@ -1201,12 +1252,12 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated report and gantt chart
</commit_message>
<xml_diff>
--- a/Documents/AI Excel sheet.xlsx
+++ b/Documents/AI Excel sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Desktop\AI-Sim-Project\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Year Two\AI\AI Project\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7647DF30-964C-40F1-B88C-102EE89B7253}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DDC705-0817-4F81-85B0-9A3C57FB1212}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{4885B63F-A160-4F03-8E80-DC62420CED2B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{4885B63F-A160-4F03-8E80-DC62420CED2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
   <si>
     <t>Date</t>
   </si>
@@ -228,6 +228,24 @@
   </si>
   <si>
     <t>Create OOP FSM</t>
+  </si>
+  <si>
+    <t>Create Collect Consumables State</t>
+  </si>
+  <si>
+    <t>Create Defend Base State</t>
+  </si>
+  <si>
+    <t>Create Find Cover State</t>
+  </si>
+  <si>
+    <t>Create Attack Enemy State</t>
+  </si>
+  <si>
+    <t>Create Patrol State</t>
+  </si>
+  <si>
+    <t>Creating Idle State</t>
   </si>
 </sst>
 </file>
@@ -337,7 +355,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -447,6 +465,42 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008080"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF663300"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000066"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF336600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC9900"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -541,7 +595,7 @@
     <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="20" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -574,6 +628,12 @@
     <xf numFmtId="0" fontId="8" fillId="14" borderId="2" xfId="4"/>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="5" xfId="10" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="5" xfId="10" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="60% - Accent5" xfId="8" builtinId="48"/>
@@ -592,6 +652,12 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCC9900"/>
+      <color rgb="FF336600"/>
+      <color rgb="FFFF00FF"/>
+      <color rgb="FF000066"/>
+      <color rgb="FF663300"/>
+      <color rgb="FF008080"/>
       <color rgb="FFCC00FF"/>
       <color rgb="FF00FFFF"/>
       <color rgb="FF33CC33"/>
@@ -905,10 +971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54ACA6E1-9905-41FB-A868-8339E0F1C052}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,6 +1107,17 @@
       <c r="F9" s="1"/>
       <c r="G9" s="3"/>
     </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>43896</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1050,7 +1127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB5E907D-8933-443F-B74A-7A0D16E3D46A}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1273,15 +1350,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FB6555C-7E04-40C4-8EBB-2A31159105C2}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="4" width="18.140625" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
@@ -1402,56 +1479,58 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="E7" s="32"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="13"/>
+      <c r="E8" s="33"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="13"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
+      <c r="A10" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="F10" s="35"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
@@ -1459,12 +1538,14 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
+      <c r="A11" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -1472,12 +1553,14 @@
       <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
+      <c r="A12" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="F12" s="37"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -1485,42 +1568,48 @@
       <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+      <c r="A13" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
+      <c r="A14" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="E14" s="13"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="13"/>
       <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
+      <c r="A15" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
       <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1601,6 +1690,84 @@
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
     </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>